<commit_message>
Implemented cross correlation function for comparison of experimental and simulation data in the time and frequency domains
</commit_message>
<xml_diff>
--- a/Depth Damaged States Second Crack Pipe 4/PCs at A'.xlsx
+++ b/Depth Damaged States Second Crack Pipe 4/PCs at A'.xlsx
@@ -396,10 +396,10 @@
         <v>7000</v>
       </c>
       <c r="B2">
-        <v>-0.04786588688144126</v>
+        <v>-0.04786595968153414</v>
       </c>
       <c r="C2">
-        <v>0.03125453352181239</v>
+        <v>0.03129906175051938</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>7333.333333333333</v>
       </c>
       <c r="B3">
-        <v>0.002062411654729663</v>
+        <v>0.002062426565549203</v>
       </c>
       <c r="C3">
-        <v>-0.04216035878540582</v>
+        <v>-0.04215359547223458</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>7666.666666666667</v>
       </c>
       <c r="B4">
-        <v>-0.008389223222291983</v>
+        <v>-0.008388902741605222</v>
       </c>
       <c r="C4">
-        <v>0.1131091236008533</v>
+        <v>0.1134143325068366</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +429,10 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>0.03229928875878826</v>
+        <v>0.03229928552654197</v>
       </c>
       <c r="C5">
-        <v>-0.06258426140078363</v>
+        <v>-0.06258285824168246</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +440,10 @@
         <v>8333.333333333334</v>
       </c>
       <c r="B6">
-        <v>0.07420159290377025</v>
+        <v>0.07420142915208235</v>
       </c>
       <c r="C6">
-        <v>-0.3117310691756951</v>
+        <v>-0.3118704261340687</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +451,10 @@
         <v>8666.666666666666</v>
       </c>
       <c r="B7">
-        <v>0.6318232931125201</v>
+        <v>0.6318231897019027</v>
       </c>
       <c r="C7">
-        <v>-0.1906672407806477</v>
+        <v>-0.1907309039933736</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +462,10 @@
         <v>9000</v>
       </c>
       <c r="B8">
-        <v>0.4923465686418843</v>
+        <v>0.4923464435784665</v>
       </c>
       <c r="C8">
-        <v>-0.01985422263577167</v>
+        <v>-0.01991323185584454</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +473,10 @@
         <v>9333.333333333334</v>
       </c>
       <c r="B9">
-        <v>0.1919713813426212</v>
+        <v>0.1919715138500816</v>
       </c>
       <c r="C9">
-        <v>0.01372600887395242</v>
+        <v>0.01376782324834491</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +484,10 @@
         <v>9666.666666666666</v>
       </c>
       <c r="B10">
-        <v>0.2242360232490398</v>
+        <v>0.2242362110462203</v>
       </c>
       <c r="C10">
-        <v>-0.4511446369943853</v>
+        <v>-0.4510063236255152</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,10 +495,10 @@
         <v>10000</v>
       </c>
       <c r="B11">
-        <v>-0.4320654910196223</v>
+        <v>-0.4320655539855372</v>
       </c>
       <c r="C11">
-        <v>-0.5870844539193136</v>
+        <v>-0.5870596033765908</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10333.33333333333</v>
       </c>
       <c r="B12">
-        <v>-0.1880937830116187</v>
+        <v>-0.188093914335566</v>
       </c>
       <c r="C12">
-        <v>-0.3451669108372799</v>
+        <v>-0.3453496357891911</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
         <v>10666.66666666667</v>
       </c>
       <c r="B13">
-        <v>-0.04486715217104361</v>
+        <v>-0.04486683484195093</v>
       </c>
       <c r="C13">
-        <v>-0.1172069317901746</v>
+        <v>-0.1171306652689101</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +528,10 @@
         <v>11000</v>
       </c>
       <c r="B14">
-        <v>0.08991869769868971</v>
+        <v>0.08991878087171841</v>
       </c>
       <c r="C14">
-        <v>-0.2160779217356467</v>
+        <v>-0.2160706475595034</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +539,10 @@
         <v>11333.33333333333</v>
       </c>
       <c r="B15">
-        <v>0.1360737397106739</v>
+        <v>0.1360738248358452</v>
       </c>
       <c r="C15">
-        <v>-0.09845322253580494</v>
+        <v>-0.09842774868375141</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +550,10 @@
         <v>11666.66666666667</v>
       </c>
       <c r="B16">
-        <v>0.08111050911124561</v>
+        <v>0.08111060580533799</v>
       </c>
       <c r="C16">
-        <v>-0.2939294105453309</v>
+        <v>-0.293750050706952</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +561,10 @@
         <v>12000</v>
       </c>
       <c r="B17">
-        <v>0.07135271870426649</v>
+        <v>0.07135280583911714</v>
       </c>
       <c r="C17">
-        <v>-0.1502259651332627</v>
+        <v>-0.150137282753129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CNN Modeling now Online
</commit_message>
<xml_diff>
--- a/Depth Damaged States Second Crack Pipe 4/PCs at A'.xlsx
+++ b/Depth Damaged States Second Crack Pipe 4/PCs at A'.xlsx
@@ -396,10 +396,10 @@
         <v>7000</v>
       </c>
       <c r="B2">
-        <v>-0.04786595968153414</v>
+        <v>-0.04786603907958741</v>
       </c>
       <c r="C2">
-        <v>0.03129906175051938</v>
+        <v>0.03118848714737271</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>7333.333333333333</v>
       </c>
       <c r="B3">
-        <v>0.002062426565549203</v>
+        <v>0.002062552470441211</v>
       </c>
       <c r="C3">
-        <v>-0.04215359547223458</v>
+        <v>-0.04210452156519791</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>7666.666666666667</v>
       </c>
       <c r="B4">
-        <v>-0.008388902741605222</v>
+        <v>-0.008389029033924102</v>
       </c>
       <c r="C4">
-        <v>0.1134143325068366</v>
+        <v>0.113371726113103</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +429,10 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>0.03229928552654197</v>
+        <v>0.03229923534424699</v>
       </c>
       <c r="C5">
-        <v>-0.06258285824168246</v>
+        <v>-0.06271718936033367</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +440,10 @@
         <v>8333.333333333334</v>
       </c>
       <c r="B6">
-        <v>0.07420142915208235</v>
+        <v>0.07420144088574608</v>
       </c>
       <c r="C6">
-        <v>-0.3118704261340687</v>
+        <v>-0.3119464389254838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +451,10 @@
         <v>8666.666666666666</v>
       </c>
       <c r="B7">
-        <v>0.6318231897019027</v>
+        <v>0.6318231086506798</v>
       </c>
       <c r="C7">
-        <v>-0.1907309039933736</v>
+        <v>-0.1908208635544615</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +462,10 @@
         <v>9000</v>
       </c>
       <c r="B8">
-        <v>0.4923464435784665</v>
+        <v>0.4923464911615111</v>
       </c>
       <c r="C8">
-        <v>-0.01991323185584454</v>
+        <v>-0.01990421205148176</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +473,10 @@
         <v>9333.333333333334</v>
       </c>
       <c r="B9">
-        <v>0.1919715138500816</v>
+        <v>0.1919715282220352</v>
       </c>
       <c r="C9">
-        <v>0.01376782324834491</v>
+        <v>0.01390476784806995</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +484,10 @@
         <v>9666.666666666666</v>
       </c>
       <c r="B10">
-        <v>0.2242362110462203</v>
+        <v>0.2242362506552392</v>
       </c>
       <c r="C10">
-        <v>-0.4510063236255152</v>
+        <v>-0.4509842859865492</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,10 +495,10 @@
         <v>10000</v>
       </c>
       <c r="B11">
-        <v>-0.4320655539855372</v>
+        <v>-0.4320655373733839</v>
       </c>
       <c r="C11">
-        <v>-0.5870596033765908</v>
+        <v>-0.5870160201067577</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10333.33333333333</v>
       </c>
       <c r="B12">
-        <v>-0.188093914335566</v>
+        <v>-0.1880940029370211</v>
       </c>
       <c r="C12">
-        <v>-0.3453496357891911</v>
+        <v>-0.3454187322542644</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
         <v>10666.66666666667</v>
       </c>
       <c r="B13">
-        <v>-0.04486683484195093</v>
+        <v>-0.04486678336824379</v>
       </c>
       <c r="C13">
-        <v>-0.1171306652689101</v>
+        <v>-0.1172070204898413</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +528,10 @@
         <v>11000</v>
       </c>
       <c r="B14">
-        <v>0.08991878087171841</v>
+        <v>0.08991865304943779</v>
       </c>
       <c r="C14">
-        <v>-0.2160706475595034</v>
+        <v>-0.2162603540561481</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +539,10 @@
         <v>11333.33333333333</v>
       </c>
       <c r="B15">
-        <v>0.1360738248358452</v>
+        <v>0.1360739075037319</v>
       </c>
       <c r="C15">
-        <v>-0.09842774868375141</v>
+        <v>-0.09824363859972754</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +550,10 @@
         <v>11666.66666666667</v>
       </c>
       <c r="B16">
-        <v>0.08111060580533799</v>
+        <v>0.08111059497224249</v>
       </c>
       <c r="C16">
-        <v>-0.293750050706952</v>
+        <v>-0.2935942456603989</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +561,10 @@
         <v>12000</v>
       </c>
       <c r="B17">
-        <v>0.07135280583911714</v>
+        <v>0.0713528859684858</v>
       </c>
       <c r="C17">
-        <v>-0.150137282753129</v>
+        <v>-0.1500367814841176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>